<commit_message>
fix json unicode escaping
</commit_message>
<xml_diff>
--- a/test/sample.xlsx
+++ b/test/sample.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusuke.okada/GoogleDrive/projects/xlsxconverter/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15400" yWindow="3400" windowWidth="32740" windowHeight="23860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25600" yWindow="-4060" windowWidth="32740" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="dummy1" sheetId="2" r:id="rId1"/>
@@ -14,6 +19,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="336">
   <si>
     <t>連番</t>
   </si>
@@ -940,10 +948,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ひひひ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>アアア</t>
   </si>
   <si>
@@ -1007,9 +1011,6 @@
     <t>サササ</t>
   </si>
   <si>
-    <t>ヒヒヒ</t>
-  </si>
-  <si>
     <t>aaa</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1094,10 +1095,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>hihihi</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>なまえ</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1119,6 +1116,13 @@
   </si>
   <si>
     <t>現住都道府県</t>
+  </si>
+  <si>
+    <t>¥１００</t>
+  </si>
+  <si>
+    <t>hyakuyen</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1179,12 +1183,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1217,12 +1236,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1255,6 +1277,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1582,17 +1609,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:V16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5:R8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="16" max="16" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1660,7 +1687,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1671,16 +1698,16 @@
         <v>276</v>
       </c>
       <c r="D6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E6" t="s">
         <v>287</v>
       </c>
-      <c r="E6" t="s">
-        <v>288</v>
-      </c>
       <c r="F6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H6" t="s">
         <v>17</v>
@@ -1725,7 +1752,7 @@
         <v>16256</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1736,16 +1763,16 @@
         <v>277</v>
       </c>
       <c r="D7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E7" t="s">
         <v>289</v>
       </c>
-      <c r="E7" t="s">
-        <v>290</v>
-      </c>
       <c r="F7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H7" t="s">
         <v>27</v>
@@ -1793,7 +1820,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1804,16 +1831,16 @@
         <v>278</v>
       </c>
       <c r="D8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E8" t="s">
         <v>291</v>
       </c>
-      <c r="E8" t="s">
-        <v>292</v>
-      </c>
       <c r="F8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H8" t="s">
         <v>17</v>
@@ -1861,7 +1888,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -1872,16 +1899,16 @@
         <v>279</v>
       </c>
       <c r="D9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E9" t="s">
         <v>293</v>
       </c>
-      <c r="E9" t="s">
-        <v>294</v>
-      </c>
       <c r="F9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H9" t="s">
         <v>17</v>
@@ -1929,7 +1956,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -1940,16 +1967,16 @@
         <v>280</v>
       </c>
       <c r="D10" t="s">
+        <v>294</v>
+      </c>
+      <c r="E10" t="s">
         <v>295</v>
       </c>
-      <c r="E10" t="s">
-        <v>296</v>
-      </c>
       <c r="F10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G10" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H10" t="s">
         <v>17</v>
@@ -1997,7 +2024,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>6</v>
       </c>
@@ -2008,16 +2035,16 @@
         <v>281</v>
       </c>
       <c r="D11" t="s">
+        <v>296</v>
+      </c>
+      <c r="E11" t="s">
         <v>297</v>
       </c>
-      <c r="E11" t="s">
-        <v>298</v>
-      </c>
       <c r="F11" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G11" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H11" t="s">
         <v>17</v>
@@ -2065,7 +2092,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>7</v>
       </c>
@@ -2076,16 +2103,16 @@
         <v>282</v>
       </c>
       <c r="D12" t="s">
+        <v>298</v>
+      </c>
+      <c r="E12" t="s">
         <v>299</v>
       </c>
-      <c r="E12" t="s">
-        <v>300</v>
-      </c>
       <c r="F12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H12" t="s">
         <v>27</v>
@@ -2130,7 +2157,7 @@
         <v>62829</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>8</v>
       </c>
@@ -2141,16 +2168,16 @@
         <v>283</v>
       </c>
       <c r="D13" t="s">
+        <v>300</v>
+      </c>
+      <c r="E13" t="s">
         <v>301</v>
       </c>
-      <c r="E13" t="s">
-        <v>302</v>
-      </c>
       <c r="F13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
@@ -2198,7 +2225,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>9</v>
       </c>
@@ -2209,16 +2236,16 @@
         <v>284</v>
       </c>
       <c r="D14" t="s">
+        <v>302</v>
+      </c>
+      <c r="E14" t="s">
         <v>303</v>
       </c>
-      <c r="E14" t="s">
-        <v>304</v>
-      </c>
       <c r="F14" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H14" t="s">
         <v>27</v>
@@ -2266,7 +2293,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>10</v>
       </c>
@@ -2277,16 +2304,16 @@
         <v>285</v>
       </c>
       <c r="D15" t="s">
+        <v>304</v>
+      </c>
+      <c r="E15" t="s">
         <v>305</v>
       </c>
-      <c r="E15" t="s">
-        <v>306</v>
-      </c>
       <c r="F15" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G15" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H15" t="s">
         <v>27</v>
@@ -2331,27 +2358,27 @@
         <v>33602</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>275</v>
       </c>
-      <c r="C16" t="s">
-        <v>286</v>
+      <c r="C16" s="5" t="s">
+        <v>334</v>
       </c>
       <c r="D16" t="s">
-        <v>307</v>
-      </c>
-      <c r="E16" t="s">
-        <v>308</v>
+        <v>306</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>334</v>
       </c>
       <c r="F16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G16" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="H16" t="s">
         <v>27</v>
@@ -2403,11 +2430,6 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2415,13 +2437,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2435,10 +2457,10 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -2452,10 +2474,10 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -2469,10 +2491,10 @@
         <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -2486,18 +2508,13 @@
         <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2509,9 +2526,9 @@
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2525,7 +2542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -2539,7 +2556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -2550,10 +2567,10 @@
         <v>277</v>
       </c>
       <c r="D7" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -2571,11 +2588,6 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2587,9 +2599,9 @@
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>252</v>
       </c>
@@ -2597,7 +2609,7 @@
         <v>253</v>
       </c>
       <c r="C5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D5" t="s">
         <v>254</v>
@@ -2606,7 +2618,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2623,7 +2635,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2640,7 +2652,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2657,7 +2669,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2674,7 +2686,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>5</v>
       </c>
@@ -2691,7 +2703,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>6</v>
       </c>
@@ -2708,7 +2720,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>7</v>
       </c>
@@ -2725,7 +2737,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>8</v>
       </c>
@@ -2742,7 +2754,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>9</v>
       </c>
@@ -2759,7 +2771,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>10</v>
       </c>
@@ -2776,7 +2788,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>11</v>
       </c>
@@ -2790,7 +2802,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>12</v>
       </c>
@@ -2807,7 +2819,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>13</v>
       </c>
@@ -2824,7 +2836,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>14</v>
       </c>
@@ -2841,7 +2853,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>15</v>
       </c>
@@ -2858,7 +2870,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>16</v>
       </c>
@@ -2875,7 +2887,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>17</v>
       </c>
@@ -2892,7 +2904,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>18</v>
       </c>
@@ -2909,7 +2921,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>19</v>
       </c>
@@ -2926,7 +2938,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>20</v>
       </c>
@@ -2943,7 +2955,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>21</v>
       </c>
@@ -2960,7 +2972,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>22</v>
       </c>
@@ -2977,7 +2989,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>23</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>24</v>
       </c>
@@ -3011,7 +3023,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>25</v>
       </c>
@@ -3028,7 +3040,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>26</v>
       </c>
@@ -3045,7 +3057,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>27</v>
       </c>
@@ -3062,7 +3074,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>28</v>
       </c>
@@ -3079,7 +3091,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>29</v>
       </c>
@@ -3096,7 +3108,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>30</v>
       </c>
@@ -3113,7 +3125,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>31</v>
       </c>
@@ -3130,7 +3142,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>32</v>
       </c>
@@ -3147,7 +3159,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>33</v>
       </c>
@@ -3164,7 +3176,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>34</v>
       </c>
@@ -3181,7 +3193,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>35</v>
       </c>
@@ -3198,7 +3210,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>36</v>
       </c>
@@ -3215,7 +3227,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>37</v>
       </c>
@@ -3232,7 +3244,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>38</v>
       </c>
@@ -3249,7 +3261,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>39</v>
       </c>
@@ -3266,7 +3278,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>40</v>
       </c>
@@ -3283,7 +3295,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>41</v>
       </c>
@@ -3300,7 +3312,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>42</v>
       </c>
@@ -3317,7 +3329,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>43</v>
       </c>
@@ -3334,7 +3346,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>44</v>
       </c>
@@ -3351,7 +3363,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>45</v>
       </c>
@@ -3368,7 +3380,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>46</v>
       </c>
@@ -3385,7 +3397,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>47</v>
       </c>
@@ -3405,10 +3417,5 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
support rowx,colx <-> cellname
</commit_message>
<xml_diff>
--- a/test/sample.xlsx
+++ b/test/sample.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-4060" windowWidth="32740" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="35120" yWindow="-360" windowWidth="19800" windowHeight="13580" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="dummy1" sheetId="2" r:id="rId1"/>
     <sheet name="dummy2" sheetId="5" r:id="rId2"/>
     <sheet name="nothing_foreignkey" sheetId="4" r:id="rId3"/>
     <sheet name="都道府県" sheetId="3" r:id="rId4"/>
+    <sheet name="test" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="392">
   <si>
     <t>連番</t>
   </si>
@@ -1338,6 +1339,14 @@
   </si>
   <si>
     <t>出力無効</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ZZ1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AAA1</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1825,7 +1834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
@@ -3872,4 +3881,2266 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AAA10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="ZP1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="ZX12" sqref="ZX12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:703" x14ac:dyDescent="0.15">
+      <c r="A1">
+        <v>1001</v>
+      </c>
+      <c r="B1">
+        <v>1002</v>
+      </c>
+      <c r="C1">
+        <v>1003</v>
+      </c>
+      <c r="D1">
+        <v>1004</v>
+      </c>
+      <c r="E1">
+        <v>1005</v>
+      </c>
+      <c r="F1">
+        <v>1006</v>
+      </c>
+      <c r="G1">
+        <v>1007</v>
+      </c>
+      <c r="H1">
+        <v>1008</v>
+      </c>
+      <c r="I1">
+        <v>1009</v>
+      </c>
+      <c r="J1">
+        <v>1010</v>
+      </c>
+      <c r="K1">
+        <v>1011</v>
+      </c>
+      <c r="L1">
+        <v>1012</v>
+      </c>
+      <c r="M1">
+        <v>1013</v>
+      </c>
+      <c r="N1">
+        <v>1014</v>
+      </c>
+      <c r="O1">
+        <v>1015</v>
+      </c>
+      <c r="P1">
+        <v>1016</v>
+      </c>
+      <c r="Q1">
+        <v>1017</v>
+      </c>
+      <c r="R1">
+        <v>1018</v>
+      </c>
+      <c r="S1">
+        <v>1019</v>
+      </c>
+      <c r="T1">
+        <v>1020</v>
+      </c>
+      <c r="U1">
+        <v>1021</v>
+      </c>
+      <c r="V1">
+        <v>1022</v>
+      </c>
+      <c r="W1">
+        <v>1023</v>
+      </c>
+      <c r="X1">
+        <v>1024</v>
+      </c>
+      <c r="Y1">
+        <v>1025</v>
+      </c>
+      <c r="Z1">
+        <v>1026</v>
+      </c>
+      <c r="AA1">
+        <v>1027</v>
+      </c>
+      <c r="AB1">
+        <v>1028</v>
+      </c>
+      <c r="AC1">
+        <v>1029</v>
+      </c>
+      <c r="AD1">
+        <v>1030</v>
+      </c>
+      <c r="AE1">
+        <v>1031</v>
+      </c>
+      <c r="AF1">
+        <v>1032</v>
+      </c>
+      <c r="AG1">
+        <v>1033</v>
+      </c>
+      <c r="AH1">
+        <v>1034</v>
+      </c>
+      <c r="AI1">
+        <v>1035</v>
+      </c>
+      <c r="AJ1">
+        <v>1036</v>
+      </c>
+      <c r="AK1">
+        <v>1037</v>
+      </c>
+      <c r="AL1">
+        <v>1038</v>
+      </c>
+      <c r="AM1">
+        <v>1039</v>
+      </c>
+      <c r="AN1">
+        <v>1040</v>
+      </c>
+      <c r="AO1">
+        <v>1041</v>
+      </c>
+      <c r="AP1">
+        <v>1042</v>
+      </c>
+      <c r="AQ1">
+        <v>1043</v>
+      </c>
+      <c r="AR1">
+        <v>1044</v>
+      </c>
+      <c r="AS1">
+        <v>1045</v>
+      </c>
+      <c r="AT1">
+        <v>1046</v>
+      </c>
+      <c r="AU1">
+        <v>1047</v>
+      </c>
+      <c r="AV1">
+        <v>1048</v>
+      </c>
+      <c r="AW1">
+        <v>1049</v>
+      </c>
+      <c r="AX1">
+        <v>1050</v>
+      </c>
+      <c r="AY1">
+        <v>1051</v>
+      </c>
+      <c r="AZ1">
+        <v>1052</v>
+      </c>
+      <c r="BA1">
+        <v>1053</v>
+      </c>
+      <c r="BB1">
+        <v>1054</v>
+      </c>
+      <c r="BC1">
+        <v>1055</v>
+      </c>
+      <c r="BD1">
+        <v>1056</v>
+      </c>
+      <c r="BE1">
+        <v>1057</v>
+      </c>
+      <c r="BF1">
+        <v>1058</v>
+      </c>
+      <c r="BG1">
+        <v>1059</v>
+      </c>
+      <c r="BH1">
+        <v>1060</v>
+      </c>
+      <c r="BI1">
+        <v>1061</v>
+      </c>
+      <c r="BJ1">
+        <v>1062</v>
+      </c>
+      <c r="BK1">
+        <v>1063</v>
+      </c>
+      <c r="BL1">
+        <v>1064</v>
+      </c>
+      <c r="BM1">
+        <v>1065</v>
+      </c>
+      <c r="BN1">
+        <v>1066</v>
+      </c>
+      <c r="BO1">
+        <v>1067</v>
+      </c>
+      <c r="BP1">
+        <v>1068</v>
+      </c>
+      <c r="BQ1">
+        <v>1069</v>
+      </c>
+      <c r="BR1">
+        <v>1070</v>
+      </c>
+      <c r="BS1">
+        <v>1071</v>
+      </c>
+      <c r="BT1">
+        <v>1072</v>
+      </c>
+      <c r="BU1">
+        <v>1073</v>
+      </c>
+      <c r="BV1">
+        <v>1074</v>
+      </c>
+      <c r="ZZ1" t="s">
+        <v>390</v>
+      </c>
+      <c r="AAA1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:703" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>2001</v>
+      </c>
+      <c r="B2">
+        <v>2002</v>
+      </c>
+      <c r="C2">
+        <v>2003</v>
+      </c>
+      <c r="D2">
+        <v>2004</v>
+      </c>
+      <c r="E2">
+        <v>2005</v>
+      </c>
+      <c r="F2">
+        <v>2006</v>
+      </c>
+      <c r="G2">
+        <v>2007</v>
+      </c>
+      <c r="H2">
+        <v>2008</v>
+      </c>
+      <c r="I2">
+        <v>2009</v>
+      </c>
+      <c r="J2">
+        <v>2010</v>
+      </c>
+      <c r="K2">
+        <v>2011</v>
+      </c>
+      <c r="L2">
+        <v>2012</v>
+      </c>
+      <c r="M2">
+        <v>2013</v>
+      </c>
+      <c r="N2">
+        <v>2014</v>
+      </c>
+      <c r="O2">
+        <v>2015</v>
+      </c>
+      <c r="P2">
+        <v>2016</v>
+      </c>
+      <c r="Q2">
+        <v>2017</v>
+      </c>
+      <c r="R2">
+        <v>2018</v>
+      </c>
+      <c r="S2">
+        <v>2019</v>
+      </c>
+      <c r="T2">
+        <v>2020</v>
+      </c>
+      <c r="U2">
+        <v>2021</v>
+      </c>
+      <c r="V2">
+        <v>2022</v>
+      </c>
+      <c r="W2">
+        <v>2023</v>
+      </c>
+      <c r="X2">
+        <v>2024</v>
+      </c>
+      <c r="Y2">
+        <v>2025</v>
+      </c>
+      <c r="Z2">
+        <v>2026</v>
+      </c>
+      <c r="AA2">
+        <v>2027</v>
+      </c>
+      <c r="AB2">
+        <v>2028</v>
+      </c>
+      <c r="AC2">
+        <v>2029</v>
+      </c>
+      <c r="AD2">
+        <v>2030</v>
+      </c>
+      <c r="AE2">
+        <v>2031</v>
+      </c>
+      <c r="AF2">
+        <v>2032</v>
+      </c>
+      <c r="AG2">
+        <v>2033</v>
+      </c>
+      <c r="AH2">
+        <v>2034</v>
+      </c>
+      <c r="AI2">
+        <v>2035</v>
+      </c>
+      <c r="AJ2">
+        <v>2036</v>
+      </c>
+      <c r="AK2">
+        <v>2037</v>
+      </c>
+      <c r="AL2">
+        <v>2038</v>
+      </c>
+      <c r="AM2">
+        <v>2039</v>
+      </c>
+      <c r="AN2">
+        <v>2040</v>
+      </c>
+      <c r="AO2">
+        <v>2041</v>
+      </c>
+      <c r="AP2">
+        <v>2042</v>
+      </c>
+      <c r="AQ2">
+        <v>2043</v>
+      </c>
+      <c r="AR2">
+        <v>2044</v>
+      </c>
+      <c r="AS2">
+        <v>2045</v>
+      </c>
+      <c r="AT2">
+        <v>2046</v>
+      </c>
+      <c r="AU2">
+        <v>2047</v>
+      </c>
+      <c r="AV2">
+        <v>2048</v>
+      </c>
+      <c r="AW2">
+        <v>2049</v>
+      </c>
+      <c r="AX2">
+        <v>2050</v>
+      </c>
+      <c r="AY2">
+        <v>2051</v>
+      </c>
+      <c r="AZ2">
+        <v>2052</v>
+      </c>
+      <c r="BA2">
+        <v>2053</v>
+      </c>
+      <c r="BB2">
+        <v>2054</v>
+      </c>
+      <c r="BC2">
+        <v>2055</v>
+      </c>
+      <c r="BD2">
+        <v>2056</v>
+      </c>
+      <c r="BE2">
+        <v>2057</v>
+      </c>
+      <c r="BF2">
+        <v>2058</v>
+      </c>
+      <c r="BG2">
+        <v>2059</v>
+      </c>
+      <c r="BH2">
+        <v>2060</v>
+      </c>
+      <c r="BI2">
+        <v>2061</v>
+      </c>
+      <c r="BJ2">
+        <v>2062</v>
+      </c>
+      <c r="BK2">
+        <v>2063</v>
+      </c>
+      <c r="BL2">
+        <v>2064</v>
+      </c>
+      <c r="BM2">
+        <v>2065</v>
+      </c>
+      <c r="BN2">
+        <v>2066</v>
+      </c>
+      <c r="BO2">
+        <v>2067</v>
+      </c>
+      <c r="BP2">
+        <v>2068</v>
+      </c>
+      <c r="BQ2">
+        <v>2069</v>
+      </c>
+      <c r="BR2">
+        <v>2070</v>
+      </c>
+      <c r="BS2">
+        <v>2071</v>
+      </c>
+      <c r="BT2">
+        <v>2072</v>
+      </c>
+      <c r="BU2">
+        <v>2073</v>
+      </c>
+      <c r="BV2">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="3" spans="1:703" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>3001</v>
+      </c>
+      <c r="B3">
+        <v>3002</v>
+      </c>
+      <c r="C3">
+        <v>3003</v>
+      </c>
+      <c r="D3">
+        <v>3004</v>
+      </c>
+      <c r="E3">
+        <v>3005</v>
+      </c>
+      <c r="F3">
+        <v>3006</v>
+      </c>
+      <c r="G3">
+        <v>3007</v>
+      </c>
+      <c r="H3">
+        <v>3008</v>
+      </c>
+      <c r="I3">
+        <v>3009</v>
+      </c>
+      <c r="J3">
+        <v>3010</v>
+      </c>
+      <c r="K3">
+        <v>3011</v>
+      </c>
+      <c r="L3">
+        <v>3012</v>
+      </c>
+      <c r="M3">
+        <v>3013</v>
+      </c>
+      <c r="N3">
+        <v>3014</v>
+      </c>
+      <c r="O3">
+        <v>3015</v>
+      </c>
+      <c r="P3">
+        <v>3016</v>
+      </c>
+      <c r="Q3">
+        <v>3017</v>
+      </c>
+      <c r="R3">
+        <v>3018</v>
+      </c>
+      <c r="S3">
+        <v>3019</v>
+      </c>
+      <c r="T3">
+        <v>3020</v>
+      </c>
+      <c r="U3">
+        <v>3021</v>
+      </c>
+      <c r="V3">
+        <v>3022</v>
+      </c>
+      <c r="W3">
+        <v>3023</v>
+      </c>
+      <c r="X3">
+        <v>3024</v>
+      </c>
+      <c r="Y3">
+        <v>3025</v>
+      </c>
+      <c r="Z3">
+        <v>3026</v>
+      </c>
+      <c r="AA3">
+        <v>3027</v>
+      </c>
+      <c r="AB3">
+        <v>3028</v>
+      </c>
+      <c r="AC3">
+        <v>3029</v>
+      </c>
+      <c r="AD3">
+        <v>3030</v>
+      </c>
+      <c r="AE3">
+        <v>3031</v>
+      </c>
+      <c r="AF3">
+        <v>3032</v>
+      </c>
+      <c r="AG3">
+        <v>3033</v>
+      </c>
+      <c r="AH3">
+        <v>3034</v>
+      </c>
+      <c r="AI3">
+        <v>3035</v>
+      </c>
+      <c r="AJ3">
+        <v>3036</v>
+      </c>
+      <c r="AK3">
+        <v>3037</v>
+      </c>
+      <c r="AL3">
+        <v>3038</v>
+      </c>
+      <c r="AM3">
+        <v>3039</v>
+      </c>
+      <c r="AN3">
+        <v>3040</v>
+      </c>
+      <c r="AO3">
+        <v>3041</v>
+      </c>
+      <c r="AP3">
+        <v>3042</v>
+      </c>
+      <c r="AQ3">
+        <v>3043</v>
+      </c>
+      <c r="AR3">
+        <v>3044</v>
+      </c>
+      <c r="AS3">
+        <v>3045</v>
+      </c>
+      <c r="AT3">
+        <v>3046</v>
+      </c>
+      <c r="AU3">
+        <v>3047</v>
+      </c>
+      <c r="AV3">
+        <v>3048</v>
+      </c>
+      <c r="AW3">
+        <v>3049</v>
+      </c>
+      <c r="AX3">
+        <v>3050</v>
+      </c>
+      <c r="AY3">
+        <v>3051</v>
+      </c>
+      <c r="AZ3">
+        <v>3052</v>
+      </c>
+      <c r="BA3">
+        <v>3053</v>
+      </c>
+      <c r="BB3">
+        <v>3054</v>
+      </c>
+      <c r="BC3">
+        <v>3055</v>
+      </c>
+      <c r="BD3">
+        <v>3056</v>
+      </c>
+      <c r="BE3">
+        <v>3057</v>
+      </c>
+      <c r="BF3">
+        <v>3058</v>
+      </c>
+      <c r="BG3">
+        <v>3059</v>
+      </c>
+      <c r="BH3">
+        <v>3060</v>
+      </c>
+      <c r="BI3">
+        <v>3061</v>
+      </c>
+      <c r="BJ3">
+        <v>3062</v>
+      </c>
+      <c r="BK3">
+        <v>3063</v>
+      </c>
+      <c r="BL3">
+        <v>3064</v>
+      </c>
+      <c r="BM3">
+        <v>3065</v>
+      </c>
+      <c r="BN3">
+        <v>3066</v>
+      </c>
+      <c r="BO3">
+        <v>3067</v>
+      </c>
+      <c r="BP3">
+        <v>3068</v>
+      </c>
+      <c r="BQ3">
+        <v>3069</v>
+      </c>
+      <c r="BR3">
+        <v>3070</v>
+      </c>
+      <c r="BS3">
+        <v>3071</v>
+      </c>
+      <c r="BT3">
+        <v>3072</v>
+      </c>
+      <c r="BU3">
+        <v>3073</v>
+      </c>
+      <c r="BV3">
+        <v>3074</v>
+      </c>
+    </row>
+    <row r="4" spans="1:703" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>4001</v>
+      </c>
+      <c r="B4">
+        <v>4002</v>
+      </c>
+      <c r="C4">
+        <v>4003</v>
+      </c>
+      <c r="D4">
+        <v>4004</v>
+      </c>
+      <c r="E4">
+        <v>4005</v>
+      </c>
+      <c r="F4">
+        <v>4006</v>
+      </c>
+      <c r="G4">
+        <v>4007</v>
+      </c>
+      <c r="H4">
+        <v>4008</v>
+      </c>
+      <c r="I4">
+        <v>4009</v>
+      </c>
+      <c r="J4">
+        <v>4010</v>
+      </c>
+      <c r="K4">
+        <v>4011</v>
+      </c>
+      <c r="L4">
+        <v>4012</v>
+      </c>
+      <c r="M4">
+        <v>4013</v>
+      </c>
+      <c r="N4">
+        <v>4014</v>
+      </c>
+      <c r="O4">
+        <v>4015</v>
+      </c>
+      <c r="P4">
+        <v>4016</v>
+      </c>
+      <c r="Q4">
+        <v>4017</v>
+      </c>
+      <c r="R4">
+        <v>4018</v>
+      </c>
+      <c r="S4">
+        <v>4019</v>
+      </c>
+      <c r="T4">
+        <v>4020</v>
+      </c>
+      <c r="U4">
+        <v>4021</v>
+      </c>
+      <c r="V4">
+        <v>4022</v>
+      </c>
+      <c r="W4">
+        <v>4023</v>
+      </c>
+      <c r="X4">
+        <v>4024</v>
+      </c>
+      <c r="Y4">
+        <v>4025</v>
+      </c>
+      <c r="Z4">
+        <v>4026</v>
+      </c>
+      <c r="AA4">
+        <v>4027</v>
+      </c>
+      <c r="AB4">
+        <v>4028</v>
+      </c>
+      <c r="AC4">
+        <v>4029</v>
+      </c>
+      <c r="AD4">
+        <v>4030</v>
+      </c>
+      <c r="AE4">
+        <v>4031</v>
+      </c>
+      <c r="AF4">
+        <v>4032</v>
+      </c>
+      <c r="AG4">
+        <v>4033</v>
+      </c>
+      <c r="AH4">
+        <v>4034</v>
+      </c>
+      <c r="AI4">
+        <v>4035</v>
+      </c>
+      <c r="AJ4">
+        <v>4036</v>
+      </c>
+      <c r="AK4">
+        <v>4037</v>
+      </c>
+      <c r="AL4">
+        <v>4038</v>
+      </c>
+      <c r="AM4">
+        <v>4039</v>
+      </c>
+      <c r="AN4">
+        <v>4040</v>
+      </c>
+      <c r="AO4">
+        <v>4041</v>
+      </c>
+      <c r="AP4">
+        <v>4042</v>
+      </c>
+      <c r="AQ4">
+        <v>4043</v>
+      </c>
+      <c r="AR4">
+        <v>4044</v>
+      </c>
+      <c r="AS4">
+        <v>4045</v>
+      </c>
+      <c r="AT4">
+        <v>4046</v>
+      </c>
+      <c r="AU4">
+        <v>4047</v>
+      </c>
+      <c r="AV4">
+        <v>4048</v>
+      </c>
+      <c r="AW4">
+        <v>4049</v>
+      </c>
+      <c r="AX4">
+        <v>4050</v>
+      </c>
+      <c r="AY4">
+        <v>4051</v>
+      </c>
+      <c r="AZ4">
+        <v>4052</v>
+      </c>
+      <c r="BA4">
+        <v>4053</v>
+      </c>
+      <c r="BB4">
+        <v>4054</v>
+      </c>
+      <c r="BC4">
+        <v>4055</v>
+      </c>
+      <c r="BD4">
+        <v>4056</v>
+      </c>
+      <c r="BE4">
+        <v>4057</v>
+      </c>
+      <c r="BF4">
+        <v>4058</v>
+      </c>
+      <c r="BG4">
+        <v>4059</v>
+      </c>
+      <c r="BH4">
+        <v>4060</v>
+      </c>
+      <c r="BI4">
+        <v>4061</v>
+      </c>
+      <c r="BJ4">
+        <v>4062</v>
+      </c>
+      <c r="BK4">
+        <v>4063</v>
+      </c>
+      <c r="BL4">
+        <v>4064</v>
+      </c>
+      <c r="BM4">
+        <v>4065</v>
+      </c>
+      <c r="BN4">
+        <v>4066</v>
+      </c>
+      <c r="BO4">
+        <v>4067</v>
+      </c>
+      <c r="BP4">
+        <v>4068</v>
+      </c>
+      <c r="BQ4">
+        <v>4069</v>
+      </c>
+      <c r="BR4">
+        <v>4070</v>
+      </c>
+      <c r="BS4">
+        <v>4071</v>
+      </c>
+      <c r="BT4">
+        <v>4072</v>
+      </c>
+      <c r="BU4">
+        <v>4073</v>
+      </c>
+      <c r="BV4">
+        <v>4074</v>
+      </c>
+    </row>
+    <row r="5" spans="1:703" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>5001</v>
+      </c>
+      <c r="B5">
+        <v>5002</v>
+      </c>
+      <c r="C5">
+        <v>5003</v>
+      </c>
+      <c r="D5">
+        <v>5004</v>
+      </c>
+      <c r="E5">
+        <v>5005</v>
+      </c>
+      <c r="F5">
+        <v>5006</v>
+      </c>
+      <c r="G5">
+        <v>5007</v>
+      </c>
+      <c r="H5">
+        <v>5008</v>
+      </c>
+      <c r="I5">
+        <v>5009</v>
+      </c>
+      <c r="J5">
+        <v>5010</v>
+      </c>
+      <c r="K5">
+        <v>5011</v>
+      </c>
+      <c r="L5">
+        <v>5012</v>
+      </c>
+      <c r="M5">
+        <v>5013</v>
+      </c>
+      <c r="N5">
+        <v>5014</v>
+      </c>
+      <c r="O5">
+        <v>5015</v>
+      </c>
+      <c r="P5">
+        <v>5016</v>
+      </c>
+      <c r="Q5">
+        <v>5017</v>
+      </c>
+      <c r="R5">
+        <v>5018</v>
+      </c>
+      <c r="S5">
+        <v>5019</v>
+      </c>
+      <c r="T5">
+        <v>5020</v>
+      </c>
+      <c r="U5">
+        <v>5021</v>
+      </c>
+      <c r="V5">
+        <v>5022</v>
+      </c>
+      <c r="W5">
+        <v>5023</v>
+      </c>
+      <c r="X5">
+        <v>5024</v>
+      </c>
+      <c r="Y5">
+        <v>5025</v>
+      </c>
+      <c r="Z5">
+        <v>5026</v>
+      </c>
+      <c r="AA5">
+        <v>5027</v>
+      </c>
+      <c r="AB5">
+        <v>5028</v>
+      </c>
+      <c r="AC5">
+        <v>5029</v>
+      </c>
+      <c r="AD5">
+        <v>5030</v>
+      </c>
+      <c r="AE5">
+        <v>5031</v>
+      </c>
+      <c r="AF5">
+        <v>5032</v>
+      </c>
+      <c r="AG5">
+        <v>5033</v>
+      </c>
+      <c r="AH5">
+        <v>5034</v>
+      </c>
+      <c r="AI5">
+        <v>5035</v>
+      </c>
+      <c r="AJ5">
+        <v>5036</v>
+      </c>
+      <c r="AK5">
+        <v>5037</v>
+      </c>
+      <c r="AL5">
+        <v>5038</v>
+      </c>
+      <c r="AM5">
+        <v>5039</v>
+      </c>
+      <c r="AN5">
+        <v>5040</v>
+      </c>
+      <c r="AO5">
+        <v>5041</v>
+      </c>
+      <c r="AP5">
+        <v>5042</v>
+      </c>
+      <c r="AQ5">
+        <v>5043</v>
+      </c>
+      <c r="AR5">
+        <v>5044</v>
+      </c>
+      <c r="AS5">
+        <v>5045</v>
+      </c>
+      <c r="AT5">
+        <v>5046</v>
+      </c>
+      <c r="AU5">
+        <v>5047</v>
+      </c>
+      <c r="AV5">
+        <v>5048</v>
+      </c>
+      <c r="AW5">
+        <v>5049</v>
+      </c>
+      <c r="AX5">
+        <v>5050</v>
+      </c>
+      <c r="AY5">
+        <v>5051</v>
+      </c>
+      <c r="AZ5">
+        <v>5052</v>
+      </c>
+      <c r="BA5">
+        <v>5053</v>
+      </c>
+      <c r="BB5">
+        <v>5054</v>
+      </c>
+      <c r="BC5">
+        <v>5055</v>
+      </c>
+      <c r="BD5">
+        <v>5056</v>
+      </c>
+      <c r="BE5">
+        <v>5057</v>
+      </c>
+      <c r="BF5">
+        <v>5058</v>
+      </c>
+      <c r="BG5">
+        <v>5059</v>
+      </c>
+      <c r="BH5">
+        <v>5060</v>
+      </c>
+      <c r="BI5">
+        <v>5061</v>
+      </c>
+      <c r="BJ5">
+        <v>5062</v>
+      </c>
+      <c r="BK5">
+        <v>5063</v>
+      </c>
+      <c r="BL5">
+        <v>5064</v>
+      </c>
+      <c r="BM5">
+        <v>5065</v>
+      </c>
+      <c r="BN5">
+        <v>5066</v>
+      </c>
+      <c r="BO5">
+        <v>5067</v>
+      </c>
+      <c r="BP5">
+        <v>5068</v>
+      </c>
+      <c r="BQ5">
+        <v>5069</v>
+      </c>
+      <c r="BR5">
+        <v>5070</v>
+      </c>
+      <c r="BS5">
+        <v>5071</v>
+      </c>
+      <c r="BT5">
+        <v>5072</v>
+      </c>
+      <c r="BU5">
+        <v>5073</v>
+      </c>
+      <c r="BV5">
+        <v>5074</v>
+      </c>
+    </row>
+    <row r="6" spans="1:703" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>6001</v>
+      </c>
+      <c r="B6">
+        <v>6002</v>
+      </c>
+      <c r="C6">
+        <v>6003</v>
+      </c>
+      <c r="D6">
+        <v>6004</v>
+      </c>
+      <c r="E6">
+        <v>6005</v>
+      </c>
+      <c r="F6">
+        <v>6006</v>
+      </c>
+      <c r="G6">
+        <v>6007</v>
+      </c>
+      <c r="H6">
+        <v>6008</v>
+      </c>
+      <c r="I6">
+        <v>6009</v>
+      </c>
+      <c r="J6">
+        <v>6010</v>
+      </c>
+      <c r="K6">
+        <v>6011</v>
+      </c>
+      <c r="L6">
+        <v>6012</v>
+      </c>
+      <c r="M6">
+        <v>6013</v>
+      </c>
+      <c r="N6">
+        <v>6014</v>
+      </c>
+      <c r="O6">
+        <v>6015</v>
+      </c>
+      <c r="P6">
+        <v>6016</v>
+      </c>
+      <c r="Q6">
+        <v>6017</v>
+      </c>
+      <c r="R6">
+        <v>6018</v>
+      </c>
+      <c r="S6">
+        <v>6019</v>
+      </c>
+      <c r="T6">
+        <v>6020</v>
+      </c>
+      <c r="U6">
+        <v>6021</v>
+      </c>
+      <c r="V6">
+        <v>6022</v>
+      </c>
+      <c r="W6">
+        <v>6023</v>
+      </c>
+      <c r="X6">
+        <v>6024</v>
+      </c>
+      <c r="Y6">
+        <v>6025</v>
+      </c>
+      <c r="Z6">
+        <v>6026</v>
+      </c>
+      <c r="AA6">
+        <v>6027</v>
+      </c>
+      <c r="AB6">
+        <v>6028</v>
+      </c>
+      <c r="AC6">
+        <v>6029</v>
+      </c>
+      <c r="AD6">
+        <v>6030</v>
+      </c>
+      <c r="AE6">
+        <v>6031</v>
+      </c>
+      <c r="AF6">
+        <v>6032</v>
+      </c>
+      <c r="AG6">
+        <v>6033</v>
+      </c>
+      <c r="AH6">
+        <v>6034</v>
+      </c>
+      <c r="AI6">
+        <v>6035</v>
+      </c>
+      <c r="AJ6">
+        <v>6036</v>
+      </c>
+      <c r="AK6">
+        <v>6037</v>
+      </c>
+      <c r="AL6">
+        <v>6038</v>
+      </c>
+      <c r="AM6">
+        <v>6039</v>
+      </c>
+      <c r="AN6">
+        <v>6040</v>
+      </c>
+      <c r="AO6">
+        <v>6041</v>
+      </c>
+      <c r="AP6">
+        <v>6042</v>
+      </c>
+      <c r="AQ6">
+        <v>6043</v>
+      </c>
+      <c r="AR6">
+        <v>6044</v>
+      </c>
+      <c r="AS6">
+        <v>6045</v>
+      </c>
+      <c r="AT6">
+        <v>6046</v>
+      </c>
+      <c r="AU6">
+        <v>6047</v>
+      </c>
+      <c r="AV6">
+        <v>6048</v>
+      </c>
+      <c r="AW6">
+        <v>6049</v>
+      </c>
+      <c r="AX6">
+        <v>6050</v>
+      </c>
+      <c r="AY6">
+        <v>6051</v>
+      </c>
+      <c r="AZ6">
+        <v>6052</v>
+      </c>
+      <c r="BA6">
+        <v>6053</v>
+      </c>
+      <c r="BB6">
+        <v>6054</v>
+      </c>
+      <c r="BC6">
+        <v>6055</v>
+      </c>
+      <c r="BD6">
+        <v>6056</v>
+      </c>
+      <c r="BE6">
+        <v>6057</v>
+      </c>
+      <c r="BF6">
+        <v>6058</v>
+      </c>
+      <c r="BG6">
+        <v>6059</v>
+      </c>
+      <c r="BH6">
+        <v>6060</v>
+      </c>
+      <c r="BI6">
+        <v>6061</v>
+      </c>
+      <c r="BJ6">
+        <v>6062</v>
+      </c>
+      <c r="BK6">
+        <v>6063</v>
+      </c>
+      <c r="BL6">
+        <v>6064</v>
+      </c>
+      <c r="BM6">
+        <v>6065</v>
+      </c>
+      <c r="BN6">
+        <v>6066</v>
+      </c>
+      <c r="BO6">
+        <v>6067</v>
+      </c>
+      <c r="BP6">
+        <v>6068</v>
+      </c>
+      <c r="BQ6">
+        <v>6069</v>
+      </c>
+      <c r="BR6">
+        <v>6070</v>
+      </c>
+      <c r="BS6">
+        <v>6071</v>
+      </c>
+      <c r="BT6">
+        <v>6072</v>
+      </c>
+      <c r="BU6">
+        <v>6073</v>
+      </c>
+      <c r="BV6">
+        <v>6074</v>
+      </c>
+    </row>
+    <row r="7" spans="1:703" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>7001</v>
+      </c>
+      <c r="B7">
+        <v>7002</v>
+      </c>
+      <c r="C7">
+        <v>7003</v>
+      </c>
+      <c r="D7">
+        <v>7004</v>
+      </c>
+      <c r="E7">
+        <v>7005</v>
+      </c>
+      <c r="F7">
+        <v>7006</v>
+      </c>
+      <c r="G7">
+        <v>7007</v>
+      </c>
+      <c r="H7">
+        <v>7008</v>
+      </c>
+      <c r="I7">
+        <v>7009</v>
+      </c>
+      <c r="J7">
+        <v>7010</v>
+      </c>
+      <c r="K7">
+        <v>7011</v>
+      </c>
+      <c r="L7">
+        <v>7012</v>
+      </c>
+      <c r="M7">
+        <v>7013</v>
+      </c>
+      <c r="N7">
+        <v>7014</v>
+      </c>
+      <c r="O7">
+        <v>7015</v>
+      </c>
+      <c r="P7">
+        <v>7016</v>
+      </c>
+      <c r="Q7">
+        <v>7017</v>
+      </c>
+      <c r="R7">
+        <v>7018</v>
+      </c>
+      <c r="S7">
+        <v>7019</v>
+      </c>
+      <c r="T7">
+        <v>7020</v>
+      </c>
+      <c r="U7">
+        <v>7021</v>
+      </c>
+      <c r="V7">
+        <v>7022</v>
+      </c>
+      <c r="W7">
+        <v>7023</v>
+      </c>
+      <c r="X7">
+        <v>7024</v>
+      </c>
+      <c r="Y7">
+        <v>7025</v>
+      </c>
+      <c r="Z7">
+        <v>7026</v>
+      </c>
+      <c r="AA7">
+        <v>7027</v>
+      </c>
+      <c r="AB7">
+        <v>7028</v>
+      </c>
+      <c r="AC7">
+        <v>7029</v>
+      </c>
+      <c r="AD7">
+        <v>7030</v>
+      </c>
+      <c r="AE7">
+        <v>7031</v>
+      </c>
+      <c r="AF7">
+        <v>7032</v>
+      </c>
+      <c r="AG7">
+        <v>7033</v>
+      </c>
+      <c r="AH7">
+        <v>7034</v>
+      </c>
+      <c r="AI7">
+        <v>7035</v>
+      </c>
+      <c r="AJ7">
+        <v>7036</v>
+      </c>
+      <c r="AK7">
+        <v>7037</v>
+      </c>
+      <c r="AL7">
+        <v>7038</v>
+      </c>
+      <c r="AM7">
+        <v>7039</v>
+      </c>
+      <c r="AN7">
+        <v>7040</v>
+      </c>
+      <c r="AO7">
+        <v>7041</v>
+      </c>
+      <c r="AP7">
+        <v>7042</v>
+      </c>
+      <c r="AQ7">
+        <v>7043</v>
+      </c>
+      <c r="AR7">
+        <v>7044</v>
+      </c>
+      <c r="AS7">
+        <v>7045</v>
+      </c>
+      <c r="AT7">
+        <v>7046</v>
+      </c>
+      <c r="AU7">
+        <v>7047</v>
+      </c>
+      <c r="AV7">
+        <v>7048</v>
+      </c>
+      <c r="AW7">
+        <v>7049</v>
+      </c>
+      <c r="AX7">
+        <v>7050</v>
+      </c>
+      <c r="AY7">
+        <v>7051</v>
+      </c>
+      <c r="AZ7">
+        <v>7052</v>
+      </c>
+      <c r="BA7">
+        <v>7053</v>
+      </c>
+      <c r="BB7">
+        <v>7054</v>
+      </c>
+      <c r="BC7">
+        <v>7055</v>
+      </c>
+      <c r="BD7">
+        <v>7056</v>
+      </c>
+      <c r="BE7">
+        <v>7057</v>
+      </c>
+      <c r="BF7">
+        <v>7058</v>
+      </c>
+      <c r="BG7">
+        <v>7059</v>
+      </c>
+      <c r="BH7">
+        <v>7060</v>
+      </c>
+      <c r="BI7">
+        <v>7061</v>
+      </c>
+      <c r="BJ7">
+        <v>7062</v>
+      </c>
+      <c r="BK7">
+        <v>7063</v>
+      </c>
+      <c r="BL7">
+        <v>7064</v>
+      </c>
+      <c r="BM7">
+        <v>7065</v>
+      </c>
+      <c r="BN7">
+        <v>7066</v>
+      </c>
+      <c r="BO7">
+        <v>7067</v>
+      </c>
+      <c r="BP7">
+        <v>7068</v>
+      </c>
+      <c r="BQ7">
+        <v>7069</v>
+      </c>
+      <c r="BR7">
+        <v>7070</v>
+      </c>
+      <c r="BS7">
+        <v>7071</v>
+      </c>
+      <c r="BT7">
+        <v>7072</v>
+      </c>
+      <c r="BU7">
+        <v>7073</v>
+      </c>
+      <c r="BV7">
+        <v>7074</v>
+      </c>
+    </row>
+    <row r="8" spans="1:703" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>8001</v>
+      </c>
+      <c r="B8">
+        <v>8002</v>
+      </c>
+      <c r="C8">
+        <v>8003</v>
+      </c>
+      <c r="D8">
+        <v>8004</v>
+      </c>
+      <c r="E8">
+        <v>8005</v>
+      </c>
+      <c r="F8">
+        <v>8006</v>
+      </c>
+      <c r="G8">
+        <v>8007</v>
+      </c>
+      <c r="H8">
+        <v>8008</v>
+      </c>
+      <c r="I8">
+        <v>8009</v>
+      </c>
+      <c r="J8">
+        <v>8010</v>
+      </c>
+      <c r="K8">
+        <v>8011</v>
+      </c>
+      <c r="L8">
+        <v>8012</v>
+      </c>
+      <c r="M8">
+        <v>8013</v>
+      </c>
+      <c r="N8">
+        <v>8014</v>
+      </c>
+      <c r="O8">
+        <v>8015</v>
+      </c>
+      <c r="P8">
+        <v>8016</v>
+      </c>
+      <c r="Q8">
+        <v>8017</v>
+      </c>
+      <c r="R8">
+        <v>8018</v>
+      </c>
+      <c r="S8">
+        <v>8019</v>
+      </c>
+      <c r="T8">
+        <v>8020</v>
+      </c>
+      <c r="U8">
+        <v>8021</v>
+      </c>
+      <c r="V8">
+        <v>8022</v>
+      </c>
+      <c r="W8">
+        <v>8023</v>
+      </c>
+      <c r="X8">
+        <v>8024</v>
+      </c>
+      <c r="Y8">
+        <v>8025</v>
+      </c>
+      <c r="Z8">
+        <v>8026</v>
+      </c>
+      <c r="AA8">
+        <v>8027</v>
+      </c>
+      <c r="AB8">
+        <v>8028</v>
+      </c>
+      <c r="AC8">
+        <v>8029</v>
+      </c>
+      <c r="AD8">
+        <v>8030</v>
+      </c>
+      <c r="AE8">
+        <v>8031</v>
+      </c>
+      <c r="AF8">
+        <v>8032</v>
+      </c>
+      <c r="AG8">
+        <v>8033</v>
+      </c>
+      <c r="AH8">
+        <v>8034</v>
+      </c>
+      <c r="AI8">
+        <v>8035</v>
+      </c>
+      <c r="AJ8">
+        <v>8036</v>
+      </c>
+      <c r="AK8">
+        <v>8037</v>
+      </c>
+      <c r="AL8">
+        <v>8038</v>
+      </c>
+      <c r="AM8">
+        <v>8039</v>
+      </c>
+      <c r="AN8">
+        <v>8040</v>
+      </c>
+      <c r="AO8">
+        <v>8041</v>
+      </c>
+      <c r="AP8">
+        <v>8042</v>
+      </c>
+      <c r="AQ8">
+        <v>8043</v>
+      </c>
+      <c r="AR8">
+        <v>8044</v>
+      </c>
+      <c r="AS8">
+        <v>8045</v>
+      </c>
+      <c r="AT8">
+        <v>8046</v>
+      </c>
+      <c r="AU8">
+        <v>8047</v>
+      </c>
+      <c r="AV8">
+        <v>8048</v>
+      </c>
+      <c r="AW8">
+        <v>8049</v>
+      </c>
+      <c r="AX8">
+        <v>8050</v>
+      </c>
+      <c r="AY8">
+        <v>8051</v>
+      </c>
+      <c r="AZ8">
+        <v>8052</v>
+      </c>
+      <c r="BA8">
+        <v>8053</v>
+      </c>
+      <c r="BB8">
+        <v>8054</v>
+      </c>
+      <c r="BC8">
+        <v>8055</v>
+      </c>
+      <c r="BD8">
+        <v>8056</v>
+      </c>
+      <c r="BE8">
+        <v>8057</v>
+      </c>
+      <c r="BF8">
+        <v>8058</v>
+      </c>
+      <c r="BG8">
+        <v>8059</v>
+      </c>
+      <c r="BH8">
+        <v>8060</v>
+      </c>
+      <c r="BI8">
+        <v>8061</v>
+      </c>
+      <c r="BJ8">
+        <v>8062</v>
+      </c>
+      <c r="BK8">
+        <v>8063</v>
+      </c>
+      <c r="BL8">
+        <v>8064</v>
+      </c>
+      <c r="BM8">
+        <v>8065</v>
+      </c>
+      <c r="BN8">
+        <v>8066</v>
+      </c>
+      <c r="BO8">
+        <v>8067</v>
+      </c>
+      <c r="BP8">
+        <v>8068</v>
+      </c>
+      <c r="BQ8">
+        <v>8069</v>
+      </c>
+      <c r="BR8">
+        <v>8070</v>
+      </c>
+      <c r="BS8">
+        <v>8071</v>
+      </c>
+      <c r="BT8">
+        <v>8072</v>
+      </c>
+      <c r="BU8">
+        <v>8073</v>
+      </c>
+      <c r="BV8">
+        <v>8074</v>
+      </c>
+    </row>
+    <row r="9" spans="1:703" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>9001</v>
+      </c>
+      <c r="B9">
+        <v>9002</v>
+      </c>
+      <c r="C9">
+        <v>9003</v>
+      </c>
+      <c r="D9">
+        <v>9004</v>
+      </c>
+      <c r="E9">
+        <v>9005</v>
+      </c>
+      <c r="F9">
+        <v>9006</v>
+      </c>
+      <c r="G9">
+        <v>9007</v>
+      </c>
+      <c r="H9">
+        <v>9008</v>
+      </c>
+      <c r="I9">
+        <v>9009</v>
+      </c>
+      <c r="J9">
+        <v>9010</v>
+      </c>
+      <c r="K9">
+        <v>9011</v>
+      </c>
+      <c r="L9">
+        <v>9012</v>
+      </c>
+      <c r="M9">
+        <v>9013</v>
+      </c>
+      <c r="N9">
+        <v>9014</v>
+      </c>
+      <c r="O9">
+        <v>9015</v>
+      </c>
+      <c r="P9">
+        <v>9016</v>
+      </c>
+      <c r="Q9">
+        <v>9017</v>
+      </c>
+      <c r="R9">
+        <v>9018</v>
+      </c>
+      <c r="S9">
+        <v>9019</v>
+      </c>
+      <c r="T9">
+        <v>9020</v>
+      </c>
+      <c r="U9">
+        <v>9021</v>
+      </c>
+      <c r="V9">
+        <v>9022</v>
+      </c>
+      <c r="W9">
+        <v>9023</v>
+      </c>
+      <c r="X9">
+        <v>9024</v>
+      </c>
+      <c r="Y9">
+        <v>9025</v>
+      </c>
+      <c r="Z9">
+        <v>9026</v>
+      </c>
+      <c r="AA9">
+        <v>9027</v>
+      </c>
+      <c r="AB9">
+        <v>9028</v>
+      </c>
+      <c r="AC9">
+        <v>9029</v>
+      </c>
+      <c r="AD9">
+        <v>9030</v>
+      </c>
+      <c r="AE9">
+        <v>9031</v>
+      </c>
+      <c r="AF9">
+        <v>9032</v>
+      </c>
+      <c r="AG9">
+        <v>9033</v>
+      </c>
+      <c r="AH9">
+        <v>9034</v>
+      </c>
+      <c r="AI9">
+        <v>9035</v>
+      </c>
+      <c r="AJ9">
+        <v>9036</v>
+      </c>
+      <c r="AK9">
+        <v>9037</v>
+      </c>
+      <c r="AL9">
+        <v>9038</v>
+      </c>
+      <c r="AM9">
+        <v>9039</v>
+      </c>
+      <c r="AN9">
+        <v>9040</v>
+      </c>
+      <c r="AO9">
+        <v>9041</v>
+      </c>
+      <c r="AP9">
+        <v>9042</v>
+      </c>
+      <c r="AQ9">
+        <v>9043</v>
+      </c>
+      <c r="AR9">
+        <v>9044</v>
+      </c>
+      <c r="AS9">
+        <v>9045</v>
+      </c>
+      <c r="AT9">
+        <v>9046</v>
+      </c>
+      <c r="AU9">
+        <v>9047</v>
+      </c>
+      <c r="AV9">
+        <v>9048</v>
+      </c>
+      <c r="AW9">
+        <v>9049</v>
+      </c>
+      <c r="AX9">
+        <v>9050</v>
+      </c>
+      <c r="AY9">
+        <v>9051</v>
+      </c>
+      <c r="AZ9">
+        <v>9052</v>
+      </c>
+      <c r="BA9">
+        <v>9053</v>
+      </c>
+      <c r="BB9">
+        <v>9054</v>
+      </c>
+      <c r="BC9">
+        <v>9055</v>
+      </c>
+      <c r="BD9">
+        <v>9056</v>
+      </c>
+      <c r="BE9">
+        <v>9057</v>
+      </c>
+      <c r="BF9">
+        <v>9058</v>
+      </c>
+      <c r="BG9">
+        <v>9059</v>
+      </c>
+      <c r="BH9">
+        <v>9060</v>
+      </c>
+      <c r="BI9">
+        <v>9061</v>
+      </c>
+      <c r="BJ9">
+        <v>9062</v>
+      </c>
+      <c r="BK9">
+        <v>9063</v>
+      </c>
+      <c r="BL9">
+        <v>9064</v>
+      </c>
+      <c r="BM9">
+        <v>9065</v>
+      </c>
+      <c r="BN9">
+        <v>9066</v>
+      </c>
+      <c r="BO9">
+        <v>9067</v>
+      </c>
+      <c r="BP9">
+        <v>9068</v>
+      </c>
+      <c r="BQ9">
+        <v>9069</v>
+      </c>
+      <c r="BR9">
+        <v>9070</v>
+      </c>
+      <c r="BS9">
+        <v>9071</v>
+      </c>
+      <c r="BT9">
+        <v>9072</v>
+      </c>
+      <c r="BU9">
+        <v>9073</v>
+      </c>
+      <c r="BV9">
+        <v>9074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:703" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>10001</v>
+      </c>
+      <c r="B10">
+        <v>10002</v>
+      </c>
+      <c r="C10">
+        <v>10003</v>
+      </c>
+      <c r="D10">
+        <v>10004</v>
+      </c>
+      <c r="E10">
+        <v>10005</v>
+      </c>
+      <c r="F10">
+        <v>10006</v>
+      </c>
+      <c r="G10">
+        <v>10007</v>
+      </c>
+      <c r="H10">
+        <v>10008</v>
+      </c>
+      <c r="I10">
+        <v>10009</v>
+      </c>
+      <c r="J10">
+        <v>10010</v>
+      </c>
+      <c r="K10">
+        <v>10011</v>
+      </c>
+      <c r="L10">
+        <v>10012</v>
+      </c>
+      <c r="M10">
+        <v>10013</v>
+      </c>
+      <c r="N10">
+        <v>10014</v>
+      </c>
+      <c r="O10">
+        <v>10015</v>
+      </c>
+      <c r="P10">
+        <v>10016</v>
+      </c>
+      <c r="Q10">
+        <v>10017</v>
+      </c>
+      <c r="R10">
+        <v>10018</v>
+      </c>
+      <c r="S10">
+        <v>10019</v>
+      </c>
+      <c r="T10">
+        <v>10020</v>
+      </c>
+      <c r="U10">
+        <v>10021</v>
+      </c>
+      <c r="V10">
+        <v>10022</v>
+      </c>
+      <c r="W10">
+        <v>10023</v>
+      </c>
+      <c r="X10">
+        <v>10024</v>
+      </c>
+      <c r="Y10">
+        <v>10025</v>
+      </c>
+      <c r="Z10">
+        <v>10026</v>
+      </c>
+      <c r="AA10">
+        <v>10027</v>
+      </c>
+      <c r="AB10">
+        <v>10028</v>
+      </c>
+      <c r="AC10">
+        <v>10029</v>
+      </c>
+      <c r="AD10">
+        <v>10030</v>
+      </c>
+      <c r="AE10">
+        <v>10031</v>
+      </c>
+      <c r="AF10">
+        <v>10032</v>
+      </c>
+      <c r="AG10">
+        <v>10033</v>
+      </c>
+      <c r="AH10">
+        <v>10034</v>
+      </c>
+      <c r="AI10">
+        <v>10035</v>
+      </c>
+      <c r="AJ10">
+        <v>10036</v>
+      </c>
+      <c r="AK10">
+        <v>10037</v>
+      </c>
+      <c r="AL10">
+        <v>10038</v>
+      </c>
+      <c r="AM10">
+        <v>10039</v>
+      </c>
+      <c r="AN10">
+        <v>10040</v>
+      </c>
+      <c r="AO10">
+        <v>10041</v>
+      </c>
+      <c r="AP10">
+        <v>10042</v>
+      </c>
+      <c r="AQ10">
+        <v>10043</v>
+      </c>
+      <c r="AR10">
+        <v>10044</v>
+      </c>
+      <c r="AS10">
+        <v>10045</v>
+      </c>
+      <c r="AT10">
+        <v>10046</v>
+      </c>
+      <c r="AU10">
+        <v>10047</v>
+      </c>
+      <c r="AV10">
+        <v>10048</v>
+      </c>
+      <c r="AW10">
+        <v>10049</v>
+      </c>
+      <c r="AX10">
+        <v>10050</v>
+      </c>
+      <c r="AY10">
+        <v>10051</v>
+      </c>
+      <c r="AZ10">
+        <v>10052</v>
+      </c>
+      <c r="BA10">
+        <v>10053</v>
+      </c>
+      <c r="BB10">
+        <v>10054</v>
+      </c>
+      <c r="BC10">
+        <v>10055</v>
+      </c>
+      <c r="BD10">
+        <v>10056</v>
+      </c>
+      <c r="BE10">
+        <v>10057</v>
+      </c>
+      <c r="BF10">
+        <v>10058</v>
+      </c>
+      <c r="BG10">
+        <v>10059</v>
+      </c>
+      <c r="BH10">
+        <v>10060</v>
+      </c>
+      <c r="BI10">
+        <v>10061</v>
+      </c>
+      <c r="BJ10">
+        <v>10062</v>
+      </c>
+      <c r="BK10">
+        <v>10063</v>
+      </c>
+      <c r="BL10">
+        <v>10064</v>
+      </c>
+      <c r="BM10">
+        <v>10065</v>
+      </c>
+      <c r="BN10">
+        <v>10066</v>
+      </c>
+      <c r="BO10">
+        <v>10067</v>
+      </c>
+      <c r="BP10">
+        <v>10068</v>
+      </c>
+      <c r="BQ10">
+        <v>10069</v>
+      </c>
+      <c r="BR10">
+        <v>10070</v>
+      </c>
+      <c r="BS10">
+        <v>10071</v>
+      </c>
+      <c r="BT10">
+        <v>10072</v>
+      </c>
+      <c r="BU10">
+        <v>10073</v>
+      </c>
+      <c r="BV10">
+        <v>10074</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>